<commit_message>
new results-template with integrated metrics
</commit_message>
<xml_diff>
--- a/uncertainty_models/UMCDF_I2.xlsx
+++ b/uncertainty_models/UMCDF_I2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\UM_I1_I2_plateforme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\uncertainty_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDC94F9-2F29-4674-8C1B-0C92866A8FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB56653-C320-4FAB-B6A6-FCA37EE39041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>